<commit_message>
Hapus provinsi di Template Import
</commit_message>
<xml_diff>
--- a/PangkalanData/public/Template/Template Bengkel Sastra dan Bahasa.xlsx
+++ b/PangkalanData/public/Template/Template Bengkel Sastra dan Bahasa.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Provinsi</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Kota</t>
   </si>
@@ -77,46 +74,38 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -147,6 +136,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -193,19 +196,20 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,13 +220,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,79 +240,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,103 +414,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,21 +445,6 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -509,6 +491,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -530,11 +521,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -552,148 +549,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1051,10 +1048,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2"/>
@@ -1072,7 +1069,7 @@
     <col min="11" max="11" width="16.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:12">
+    <row r="1" ht="25" customHeight="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1106,15 +1103,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
     </row>
     <row r="3" ht="22" customHeight="1"/>
   </sheetData>

</xml_diff>